<commit_message>
feature: Hash Join 기능 구현
- Hash Join 기능 구현
</commit_message>
<xml_diff>
--- a/src/main/resources/financial-accounting-data.xlsx
+++ b/src/main/resources/financial-accounting-data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga31\Desktop\수업\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C47B9F-92A0-4BE6-BDCC-1F2476330DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C49A3-38F5-4D7A-BF7D-81E18FFC28EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="CorporateType" sheetId="5" r:id="rId1"/>
-    <sheet name="CorporateKind" sheetId="6" r:id="rId2"/>
-    <sheet name="Entry" sheetId="1" r:id="rId3"/>
-    <sheet name="VatType" sheetId="2" r:id="rId4"/>
-    <sheet name="CashBook" sheetId="3" r:id="rId5"/>
-    <sheet name="TaxInvoice" sheetId="4" r:id="rId6"/>
+    <sheet name="PurchaseSalesSlip" sheetId="7" r:id="rId1"/>
+    <sheet name="CorporateType" sheetId="5" r:id="rId2"/>
+    <sheet name="CorporateKind" sheetId="6" r:id="rId3"/>
+    <sheet name="Entry" sheetId="1" r:id="rId4"/>
+    <sheet name="VatType" sheetId="2" r:id="rId5"/>
+    <sheet name="CashBook" sheetId="3" r:id="rId6"/>
+    <sheet name="TaxInvoice" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -366,6 +367,59 @@
   <si>
     <t>외투법인</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vatTypeId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entryId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BigDecimal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unitPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>electronicTaxInvoiceIssued</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>test24</t>
   </si>
 </sst>
 </file>
@@ -781,52 +835,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5713A9-3753-4595-AEEA-F50BD1239D80}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD804EE-B6E1-4BD9-A4F0-3CBBF1EB9562}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.69921875" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45465</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45466</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45467</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -836,20 +1018,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3FF344-99DE-406B-9665-C71397F78565}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5713A9-3753-4595-AEEA-F50BD1239D80}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.69921875" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -857,115 +1039,31 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -975,6 +1073,145 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3FF344-99DE-406B-9665-C71397F78565}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.75" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6829820-5163-451C-BDE8-9004A047D6C2}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -982,39 +1219,39 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BEFEAC-7826-45BE-81E0-0B8E7BEEC07A}">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -1033,9 +1270,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1043,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1067,7 +1304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +1312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1083,7 +1320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1091,7 +1328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +1336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1115,7 +1352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1139,7 +1376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,7 +1384,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1155,7 +1392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1400,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1171,7 +1408,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1187,7 +1424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +1432,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1203,7 +1440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1448,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1219,7 +1456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1227,7 +1464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1235,7 +1472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1251,7 +1488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -1265,7 +1502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6BB459-5620-4A1D-9826-E641F7D7F724}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1273,17 +1510,17 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.09765625" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1306,7 +1543,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -1329,7 +1566,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1352,7 +1589,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1382,7 +1619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB35329-EBCD-46FF-8FF6-8B0ADEB759EB}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -1390,22 +1627,22 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1440,7 +1677,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1475,7 +1712,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1510,7 +1747,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
feature: UniqueValidator 기능 구현
- UniqueValidator 기능 구현
- NotNullValidator 함수명 변경
</commit_message>
<xml_diff>
--- a/src/main/resources/financial-accounting-data.xlsx
+++ b/src/main/resources/financial-accounting-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga31\Desktop\수업\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C49A3-38F5-4D7A-BF7D-81E18FFC28EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB3E900-4D8C-4020-B497-7C9B81A0CD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseSalesSlip" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="99">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -413,13 +413,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test14</t>
-  </si>
-  <si>
-    <t>test24</t>
+    <t>test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
   </si>
 </sst>
 </file>
@@ -836,21 +841,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD804EE-B6E1-4BD9-A4F0-3CBBF1EB9562}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="13.25" customWidth="1"/>
-    <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="13.19921875" customWidth="1"/>
+    <col min="10" max="10" width="25.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -882,7 +887,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -914,7 +919,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -946,7 +951,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -978,7 +983,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1007,6 +1012,38 @@
         <v>3.2</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45467</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1025,13 +1062,13 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1039,7 +1076,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1047,19 +1084,19 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
@@ -1080,13 +1117,13 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1094,7 +1131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -1102,103 +1139,103 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>80</v>
       </c>
@@ -1219,39 +1256,39 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1270,9 +1307,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1280,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1296,7 +1333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1304,7 +1341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1320,7 +1357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1328,7 +1365,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1336,7 +1373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1344,7 +1381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1352,7 +1389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1360,7 +1397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1368,7 +1405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1376,7 +1413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1384,7 +1421,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1408,7 +1445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1416,7 +1453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1424,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1432,7 +1469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1440,7 +1477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1448,7 +1485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1464,7 +1501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1472,7 +1509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1480,7 +1517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -1510,17 +1547,17 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.125" customWidth="1"/>
+    <col min="7" max="7" width="11.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1543,7 +1580,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -1566,7 +1603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1589,7 +1626,7 @@
         <v>45444</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1627,22 +1664,22 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1677,7 +1714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1712,7 +1749,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1747,7 +1784,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
feature: Voucher, PurchaseSalesSlip 테이블 수정 및 기능 추가
컬럼 추가 및 등록 기능추가 테스트 완료. 다른기능 메소드 위치 선정필요.
</commit_message>
<xml_diff>
--- a/src/main/resources/financial-accounting-data.xlsx
+++ b/src/main/resources/financial-accounting-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\Development\ERPSystem\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gj156\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0423C3C4-59A5-4B1B-9A06-4C05A9FADBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{009C80FF-13A2-4E2F-8E82-5C47A442E774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{1A754DB6-FF10-4809-A0D2-9C6CDB9AA5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="BankTransaction" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="414">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2099,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7100BCC3-DB0D-47FB-B986-1202A4F8D5FF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2571,7 +2571,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5393,21 +5393,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD804EE-B6E1-4BD9-A4F0-3CBBF1EB9562}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="13.25" customWidth="1"/>
-    <col min="10" max="10" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="13.25" customWidth="1"/>
+    <col min="11" max="11" width="25.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -5418,13 +5419,13 @@
         <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>89</v>
@@ -5436,42 +5437,48 @@
         <v>89</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5481,49 +5488,52 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>45465</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>1.2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>1.3</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>1.4</v>
       </c>
-      <c r="J3" s="1" t="b">
+      <c r="K3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
         <v>45466</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>2.1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2.2000000000000002</v>
       </c>
       <c r="H4" s="1">
         <v>2.2000000000000002</v>
@@ -5531,31 +5541,34 @@
       <c r="I4" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J4" s="1" t="b">
+      <c r="J4" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K4" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
         <v>45467</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>3.1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3.2</v>
       </c>
       <c r="H5" s="1">
         <v>3.2</v>
@@ -5563,39 +5576,45 @@
       <c r="I5" s="1">
         <v>3.2</v>
       </c>
-      <c r="J5" s="1" t="b">
+      <c r="J5" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="K5" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
         <v>45467</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>4.2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>4.3</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J6" s="1" t="b">
+      <c r="K6" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>